<commit_message>
The final version of the project has been added
</commit_message>
<xml_diff>
--- a/UML_class_diagram/Description_of_the_Human_Friends_tables.xlsx
+++ b/UML_class_diagram/Description_of_the_Human_Friends_tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor/Desktop/Python/Final_assessment_of_specialisation_developer/UML_class_diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2238CF-ABF0-F947-B3A8-488106644BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6BD3F4-9206-944C-B1FC-B4C3CB4FFFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="500" windowWidth="26000" windowHeight="17500" xr2:uid="{8FDD4A45-B9F9-214D-A097-226277B5DB1B}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>animals_id</t>
   </si>
   <si>
-    <t>animal_spesies</t>
-  </si>
-  <si>
     <t>Domestic animals</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>pack_animalsId</t>
+  </si>
+  <si>
+    <t>animal_species</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
   <dimension ref="A3:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,13 +659,13 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -680,27 +680,27 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="1">
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="1">
@@ -733,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -746,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="1">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="1">
@@ -766,7 +766,7 @@
         <v>2</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -785,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="1">
@@ -795,7 +795,7 @@
         <v>2</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -837,7 +837,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -847,7 +847,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -857,42 +857,42 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="P11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -907,13 +907,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="2">
         <v>43263</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -927,13 +927,13 @@
         <v>2</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O12" s="2">
         <v>43171</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -988,7 +988,7 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -998,7 +998,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1008,42 +1008,42 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="P17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -1058,13 +1058,13 @@
         <v>1</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="2">
         <v>45065</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -1078,13 +1078,13 @@
         <v>2</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O18" s="2">
         <v>44976</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1149,7 +1149,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1159,42 +1159,42 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L23" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="P23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
@@ -1209,13 +1209,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G24" s="2">
         <v>42561</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -1229,13 +1229,13 @@
         <v>2</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O24" s="2">
         <v>42553</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -1364,7 +1364,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -1383,10 +1383,10 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -1446,7 +1446,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -1466,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>

</xml_diff>